<commit_message>
maj audit + page 2
</commit_message>
<xml_diff>
--- a/audit.xlsx
+++ b/audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt0\Desktop\Openclassroom\P4\matthieugonzalo_4_04102021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBA04BA-1F83-46A1-A493-A8EBB54B7F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1F41B-9876-4B19-A574-0E3E803CFC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="1632" windowWidth="17280" windowHeight="10656" xr2:uid="{A8D4A3D5-9B04-4480-927F-9677EEA41963}"/>
   </bookViews>
@@ -319,27 +319,6 @@
 référencer.</t>
   </si>
   <si>
-    <t>il n'y a pas de fichier 
-.htaccess</t>
-  </si>
-  <si>
-    <t>le fichier .htaccess
-permet de compresser 
-notre document pour
-le rendre plus léger
-et ainsi le charger plus
-vite.</t>
-  </si>
-  <si>
-    <t>créer un fichier .htaccess
-à la racine du site.</t>
-  </si>
-  <si>
-    <t>pour ameliorer le
-lancement du site,
-compresser le document.</t>
-  </si>
-  <si>
     <t>inscrire notre site dans la Google search console</t>
   </si>
   <si>
@@ -457,6 +436,25 @@
   </si>
   <si>
     <t>validator.w3.org</t>
+  </si>
+  <si>
+    <t>changer la couleur
+du titre de la page 2</t>
+  </si>
+  <si>
+    <t>le titre de la page 2 ne 
+ressorts pas</t>
+  </si>
+  <si>
+    <t>il faut un contraste
+suffisant entre l'image
+d'arrière plan et de premier
+plan pour que les techniques
+d'assistances soit optimum</t>
+  </si>
+  <si>
+    <t>changer la couleur
+du titre</t>
   </si>
 </sst>
 </file>
@@ -854,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E00C76-2940-4E52-B3BC-44B4250E7DB3}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +910,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -935,7 +933,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -958,7 +956,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -981,7 +979,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1004,7 +1002,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1027,7 +1025,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1050,7 +1048,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1073,7 +1071,7 @@
         <v>41</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1116,7 +1114,7 @@
         <v>49</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
@@ -1139,7 +1137,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1162,7 +1160,7 @@
         <v>57</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -1185,15 +1183,15 @@
         <v>60</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>62</v>
@@ -1202,16 +1200,16 @@
         <v>63</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1231,38 +1229,38 @@
         <v>69</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>78</v>
@@ -1277,10 +1275,10 @@
         <v>81</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1288,42 +1286,42 @@
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="G19" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="F20" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="G20" s="5" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1332,20 +1330,20 @@
     <hyperlink ref="G3" r:id="rId2" xr:uid="{3EF47786-CED7-471F-B3D9-7BA2F94C0DC6}"/>
     <hyperlink ref="G8" r:id="rId3" xr:uid="{4A14FE18-D9D9-416D-92A4-126ADB00A036}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{1C655FCA-E8C7-42F5-A4C1-16258EAA278D}"/>
-    <hyperlink ref="G17" r:id="rId5" xr:uid="{2362D27E-FFC1-44DD-8AA2-E023B608730B}"/>
-    <hyperlink ref="G16" r:id="rId6" xr:uid="{D746271D-24E2-4763-AF88-663765DE618B}"/>
+    <hyperlink ref="G16" r:id="rId5" xr:uid="{2362D27E-FFC1-44DD-8AA2-E023B608730B}"/>
+    <hyperlink ref="G15" r:id="rId6" xr:uid="{D746271D-24E2-4763-AF88-663765DE618B}"/>
     <hyperlink ref="G12" r:id="rId7" xr:uid="{5ED42868-A23A-4742-A7A5-A70941C13D99}"/>
     <hyperlink ref="G2" r:id="rId8" xr:uid="{7F5BE639-56C5-45A8-9C1A-138FD4037F6B}"/>
     <hyperlink ref="G6" r:id="rId9" xr:uid="{38214347-8AD6-4FE7-9903-C23C575CA431}"/>
-    <hyperlink ref="G15" r:id="rId10" xr:uid="{D465D3FF-773A-436F-9B63-3E2870570A94}"/>
-    <hyperlink ref="G14" r:id="rId11" xr:uid="{C87F08B8-AD2C-46FA-AEBF-30700C78C93B}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{32A47BC5-3975-42B0-9F8E-C184C355142E}"/>
-    <hyperlink ref="G7" r:id="rId13" location=":~:text=Pour%20ins%C3%A9rer%20un%20lien%2C%20on,html%22%3E%20." xr:uid="{A9357F31-6AC9-46BA-92F0-2834833F82F4}"/>
-    <hyperlink ref="G9" r:id="rId14" xr:uid="{F375D263-61C1-4E19-8CC4-237E72EB3885}"/>
-    <hyperlink ref="G11" r:id="rId15" xr:uid="{DDA89BC4-B990-4919-9E7B-85F92CF8A2B4}"/>
-    <hyperlink ref="G18" r:id="rId16" xr:uid="{2FF75DD4-2070-4B44-BEF3-C680B09C8283}"/>
-    <hyperlink ref="G19" r:id="rId17" xr:uid="{2299396B-9F8D-4E0B-85C9-0388536B6E98}"/>
-    <hyperlink ref="G20" r:id="rId18" location="textarea" xr:uid="{F7C1482F-AE90-4EA4-8105-FE5A6DA92EB0}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{C87F08B8-AD2C-46FA-AEBF-30700C78C93B}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{32A47BC5-3975-42B0-9F8E-C184C355142E}"/>
+    <hyperlink ref="G7" r:id="rId12" location=":~:text=Pour%20ins%C3%A9rer%20un%20lien%2C%20on,html%22%3E%20." xr:uid="{A9357F31-6AC9-46BA-92F0-2834833F82F4}"/>
+    <hyperlink ref="G9" r:id="rId13" xr:uid="{F375D263-61C1-4E19-8CC4-237E72EB3885}"/>
+    <hyperlink ref="G11" r:id="rId14" xr:uid="{DDA89BC4-B990-4919-9E7B-85F92CF8A2B4}"/>
+    <hyperlink ref="G17" r:id="rId15" xr:uid="{2FF75DD4-2070-4B44-BEF3-C680B09C8283}"/>
+    <hyperlink ref="G18" r:id="rId16" xr:uid="{2299396B-9F8D-4E0B-85C9-0388536B6E98}"/>
+    <hyperlink ref="G19" r:id="rId17" location="textarea" xr:uid="{F7C1482F-AE90-4EA4-8105-FE5A6DA92EB0}"/>
+    <hyperlink ref="G20" r:id="rId18" xr:uid="{77D7A71D-1807-4F35-BA32-D82AEB901F2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
maj nav page 2
</commit_message>
<xml_diff>
--- a/audit.xlsx
+++ b/audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt0\Desktop\Openclassroom\P4\matthieugonzalo_4_04102021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1F41B-9876-4B19-A574-0E3E803CFC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A04E8C-409B-4C27-9B89-F2FC79543B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="1632" windowWidth="17280" windowHeight="10656" xr2:uid="{A8D4A3D5-9B04-4480-927F-9677EEA41963}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
   <si>
     <t>Numéro</t>
   </si>
@@ -455,6 +455,23 @@
   <si>
     <t>changer la couleur
 du titre</t>
+  </si>
+  <si>
+    <t>menu de navigation
+a mettre en page</t>
+  </si>
+  <si>
+    <t>accueil et contact
+sont collés</t>
+  </si>
+  <si>
+    <t>espacer les menu
+pour le rendre lisible
+et visible</t>
+  </si>
+  <si>
+    <t>mettre une margin-left
+au menu contact</t>
   </si>
 </sst>
 </file>
@@ -850,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E00C76-2940-4E52-B3BC-44B4250E7DB3}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1323,6 +1340,29 @@
       <c r="G20" s="5" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>